<commit_message>
lots of mechanical issues but looking good with autonomy
</commit_message>
<xml_diff>
--- a/LookupTable.xlsx
+++ b/LookupTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\Desktop\Karthik\High School\11th Grade\FRC Projects\CrescendoCode2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C446F4D-AB32-4C7E-9492-CEBCF2FD437C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F6838F-396D-425A-87DE-66B96C813DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6139B100-C94D-406C-B053-BB134507D3CB}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TY (vertical offset)</t>
   </si>
@@ -46,16 +47,7 @@
     <t>Pivot Ticks</t>
   </si>
   <si>
-    <t>Percent Speed</t>
-  </si>
-  <si>
     <t>Generating Regression</t>
-  </si>
-  <si>
-    <t>Angular Velocity</t>
-  </si>
-  <si>
-    <t>TX (horizontal offset)</t>
   </si>
 </sst>
 </file>
@@ -87,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,28 +96,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -161,15 +139,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7521C299-340E-4789-83CB-17EA78D0A84C}" name="Table4" displayName="Table4" ref="A1:F20" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:F20" xr:uid="{7521C299-340E-4789-83CB-17EA78D0A84C}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{34991CBF-5E1F-4B18-A2EF-08A933F1220E}" name="TX (horizontal offset)"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7521C299-340E-4789-83CB-17EA78D0A84C}" name="Table4" displayName="Table4" ref="A1:C20" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:C20" xr:uid="{7521C299-340E-4789-83CB-17EA78D0A84C}"/>
+  <tableColumns count="3">
     <tableColumn id="7" xr3:uid="{C36DCE2E-43EE-444A-8B83-2BA852EFBC39}" name="TY (vertical offset)"/>
     <tableColumn id="2" xr3:uid="{35220475-1DE4-4865-9CF7-AC7AB5FD292B}" name="TA (area of target)"/>
     <tableColumn id="3" xr3:uid="{329E2B11-5E6E-40B4-B987-F26D594C1F4F}" name="Pivot Ticks"/>
-    <tableColumn id="6" xr3:uid="{42EC1069-E981-40F4-899F-E5BCB8D7679D}" name="Angular Velocity"/>
-    <tableColumn id="4" xr3:uid="{5EA8CE93-4F77-473D-B78E-3D8B8F29A276}" name="Percent Speed"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -472,52 +447,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDAAE60-E485-48BA-9B35-5976A1C7C65E}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>-15.154486</v>
+      </c>
+      <c r="B2">
+        <v>0.19167000000000001</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{C2BFD5E7-F275-45A2-BFD8-F392DACFB680}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C2BFD5E7-F275-45A2-BFD8-F392DACFB680}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
day one of gwinnett done, logging all code changes. Main things to do tmrw are test new auton and intaking from the source.
</commit_message>
<xml_diff>
--- a/LookupTable.xlsx
+++ b/LookupTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\Desktop\Karthik\High School\11th Grade\FRC Projects\CrescendoCode2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F6838F-396D-425A-87DE-66B96C813DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FDD31B-690B-4ADF-8D27-86F4C72719DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6139B100-C94D-406C-B053-BB134507D3CB}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -450,7 +449,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,12 +473,6 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>-15.154486</v>
-      </c>
-      <c r="B2">
-        <v>0.19167000000000001</v>
-      </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>